<commit_message>
database design baoquyen 09.04.2022
</commit_message>
<xml_diff>
--- a/lesson16-baoquyen.xlsx
+++ b/lesson16-baoquyen.xlsx
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
   <si>
-    <t>Chi tiết sản phẩm</t>
-  </si>
-  <si>
     <t>Đơn hàng</t>
   </si>
   <si>
@@ -162,6 +159,9 @@
   </si>
   <si>
     <t>Tình Trạng Đơn Hàng</t>
+  </si>
+  <si>
+    <t>Chi tiết mặt hàng</t>
   </si>
 </sst>
 </file>
@@ -541,7 +541,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,183 +551,183 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="H2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H8" s="5"/>
     </row>
@@ -735,7 +735,7 @@
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
@@ -747,7 +747,7 @@
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>

</xml_diff>